<commit_message>
started testing and specified imports in Functions
</commit_message>
<xml_diff>
--- a/BackEndFlask/Functions/sample_files/sample_roster.xlsx
+++ b/BackEndFlask/Functions/sample_files/sample_roster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisgodinez/Documents/Junior_Fall/Soft-Stud/rubricapp/BackEndFlask/Functions/sample_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8E3832-1304-8A4F-9AB6-9ECF6F887914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71C1EE3-F2D6-0A43-984C-6577238DDBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="500" windowWidth="10000" windowHeight="8740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3080" yWindow="1900" windowWidth="23240" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -693,15 +693,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>